<commit_message>
start of testing according to the xlsx
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aseve\Documents\promed-clicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9A7D4F-883E-47B5-8067-EEC8170F005C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F731D782-9A78-4CF9-90FB-BD036B42268C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6CCF5E32-90BF-4976-8CE3-9868609CAAE5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="78">
   <si>
     <t>A06.09.005</t>
   </si>
@@ -405,8 +405,8 @@
       <sheetName val="Лист2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
         <row r="1">
           <cell r="G1" t="str">
             <v>Каргина Елена Геннадьевна</v>
@@ -774,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027DBE9-90F8-4510-9A2A-0DC7F76ECC31}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,15 +790,16 @@
     <col min="6" max="6" width="9.109375" style="1"/>
     <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="19.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="str">
         <f>[1]Лист2!G1</f>
         <v>Каргина Елена Геннадьевна</v>
       </c>
       <c r="B1" s="6" t="str">
-        <f>TEXT("17.07.1973", "ДД.ММ.ГГГГ")</f>
+        <f>TEXT(N1, "ДД.ММ.ГГГГ")</f>
         <v>17.07.1973</v>
       </c>
       <c r="C1" s="7"/>
@@ -829,13 +830,16 @@
       <c r="L1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="N1" s="3">
+        <v>26862</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="str">
-        <f>TEXT("17.07.1973", "ДД.ММ.ГГГГ")</f>
+        <f t="shared" ref="B2:B24" si="0">TEXT(N2, "ДД.ММ.ГГГГ")</f>
         <v>17.07.1973</v>
       </c>
       <c r="C2" s="7"/>
@@ -854,13 +858,16 @@
       <c r="L2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="N2" s="3">
+        <v>26862</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="str">
-        <f>TEXT("17.07.1973", "ДД.ММ.ГГГГ")</f>
+        <f t="shared" si="0"/>
         <v>17.07.1973</v>
       </c>
       <c r="C3" s="7"/>
@@ -875,6 +882,516 @@
       </c>
       <c r="G3" s="8" t="s">
         <v>74</v>
+      </c>
+      <c r="N3" s="3">
+        <v>26862</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>08.08.1960</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>22136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>08.08.1960</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="3">
+        <v>22136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>08.08.1960</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="3">
+        <v>22136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.10.1953</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>19647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.10.1953</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="1">
+        <v>19647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.10.1953</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" s="1">
+        <v>19647</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.09.1957</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>21078</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.09.1957</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11" s="1">
+        <v>21078</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.09.1957</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N12" s="1">
+        <v>21078</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>03.07.1947</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>17351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>03.07.1947</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="1">
+        <v>17351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>03.07.1947</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="1">
+        <v>17351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>11.02.1958</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>21227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>11.02.1958</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17" s="1">
+        <v>21227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>11.02.1958</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18" s="1">
+        <v>21227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.12.1977</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>28474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.12.1977</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N20" s="1">
+        <v>28474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15.12.1977</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" s="1">
+        <v>28474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>17.08.1988</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>32372</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>17.08.1988</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N23" s="1">
+        <v>32372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>17.08.1988</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N24" s="1">
+        <v>32372</v>
       </c>
     </row>
   </sheetData>
@@ -888,7 +1405,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B23"/>
+      <selection activeCell="B10" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
preparing for synchronization with the xlsx
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Documents\GitHub\promed-clicker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aseve\Documents\promed-clicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E468FB92-2B16-456A-A50C-5D539C9DCDFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1702F8B5-3FB3-4039-96AE-36F4F680AF42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{6CCF5E32-90BF-4976-8CE3-9868609CAAE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6CCF5E32-90BF-4976-8CE3-9868609CAAE5}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист1 (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId3"/>
+    <sheet name="My Sheet" sheetId="4" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
+    <sheet name="Лист1 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'My Sheet'!$A$1:$H$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>A06.09.005</t>
   </si>
@@ -266,13 +270,44 @@
   </si>
   <si>
     <t>A06.01.001</t>
+  </si>
+  <si>
+    <t>КАБИНЕТ ВРАЧА-КЛИНИЦИСТА</t>
+  </si>
+  <si>
+    <t>ФАМИЛИЯ И.О ВРАЧА КЛИНИЦИСТА</t>
+  </si>
+  <si>
+    <t>КОД ДИАГНОЗА</t>
+  </si>
+  <si>
+    <t>КОД ПОСЕЩЕНИЯ</t>
+  </si>
+  <si>
+    <t>КОД УСЛУГИ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДАТА РОЖДЕНИЯ </t>
+  </si>
+  <si>
+    <t>ВВОД</t>
+  </si>
+  <si>
+    <t>ПАЦИЕНТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пидор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts/>
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,8 +322,32 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="PT Sans Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="PT Sans Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,8 +372,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -337,11 +408,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +527,93 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,680 +1020,931 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027DBE9-90F8-4510-9A2A-0DC7F76ECC31}">
-  <dimension ref="A1:N18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C91358-37E6-4149-BBCE-8F9D3F17590A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" style="1"/>
-    <col min="14" max="14" width="19.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="40.77734375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="14" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" style="15" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" style="12" customWidth="1"/>
+    <col min="8" max="13" width="8.88671875" style="12"/>
+    <col min="14" max="14" width="19.33203125" style="13" customWidth="1"/>
+    <col min="15" max="30" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:30" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="20">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s" s="22">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s" s="23">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s" s="21">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s" s="21">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s" s="35">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s" s="24">
+        <v>82</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+    </row>
+    <row r="2" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="25">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="str">
-        <f t="shared" ref="B1:B18" si="0">TEXT(N1, "ДД.ММ.ГГГГ")</f>
-        <v>15.10.1953</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="9">
+        <f t="shared" ref="B2:B19" si="0">TEXT(N2, "ДД.ММ.ГГГГ")</f>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" t="s" s="31">
         <v>69</v>
       </c>
-      <c r="F1" s="8">
+      <c r="F2" s="32">
         <v>874737</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G2" t="s" s="36">
         <v>0</v>
       </c>
-      <c r="N1" s="1">
+      <c r="H2" s="19"/>
+      <c r="N2" s="12">
         <v>19647</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.10.1953</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B3" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" t="s" s="33">
         <v>69</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F3" s="34">
         <v>874735</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G3" t="s" s="37">
         <v>75</v>
       </c>
-      <c r="N2" s="1">
+      <c r="H3" s="11"/>
+      <c r="N3" s="12">
         <v>19647</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.10.1953</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" t="s" s="33">
         <v>69</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F4" s="34">
         <v>874733</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G4" t="s" s="37">
         <v>74</v>
       </c>
-      <c r="N3" s="1">
+      <c r="H4" s="11"/>
+      <c r="N4" s="12">
         <v>19647</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.09.1957</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B5" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F5" s="34">
         <v>874737</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G5" t="s" s="37">
         <v>0</v>
       </c>
-      <c r="N4" s="1">
+      <c r="H5" s="11"/>
+      <c r="N5" s="12">
         <v>21078</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="B5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.09.1957</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="B6" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F6" s="34">
         <v>874735</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G6" t="s" s="37">
         <v>75</v>
       </c>
-      <c r="N5" s="1">
+      <c r="H6" s="11"/>
+      <c r="N6" s="12">
         <v>21078</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.09.1957</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="B7" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F7" s="34">
         <v>874733</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G7" t="s" s="37">
         <v>74</v>
       </c>
-      <c r="N6" s="1">
+      <c r="H7" s="11"/>
+      <c r="N7" s="12">
         <v>21078</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s" s="26">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>03.07.1947</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="B8" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" t="s" s="33">
         <v>71</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F8" s="34">
         <v>874737</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G8" t="s" s="37">
         <v>0</v>
       </c>
-      <c r="N7" s="1">
+      <c r="H8" s="11"/>
+      <c r="N8" s="12">
         <v>17351</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s" s="26">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>03.07.1947</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="B9" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" t="s" s="33">
         <v>71</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="34">
         <v>874735</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G9" t="s" s="37">
         <v>75</v>
       </c>
-      <c r="N8" s="1">
+      <c r="H9" s="11"/>
+      <c r="N9" s="12">
         <v>17351</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s" s="26">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>03.07.1947</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="B10" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" t="s" s="33">
         <v>71</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="34">
         <v>874733</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G10" t="s" s="37">
         <v>74</v>
       </c>
-      <c r="N9" s="1">
+      <c r="H10" s="11"/>
+      <c r="N10" s="12">
         <v>17351</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s" s="26">
         <v>24</v>
       </c>
-      <c r="B10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>11.02.1958</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="B11" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" t="s" s="33">
         <v>72</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F11" s="34">
         <v>874737</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G11" t="s" s="37">
         <v>0</v>
       </c>
-      <c r="N10" s="1">
+      <c r="H11" s="11"/>
+      <c r="N11" s="12">
         <v>21227</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s" s="26">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>11.02.1958</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="B12" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" t="s" s="33">
         <v>72</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="34">
         <v>874735</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G12" t="s" s="37">
         <v>75</v>
       </c>
-      <c r="N11" s="1">
+      <c r="H12" s="11"/>
+      <c r="N12" s="12">
         <v>21227</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s" s="26">
         <v>24</v>
       </c>
-      <c r="B12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>11.02.1958</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="B13" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" t="s" s="33">
         <v>72</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F13" s="34">
         <v>874733</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G13" t="s" s="37">
         <v>74</v>
       </c>
-      <c r="N12" s="1">
+      <c r="H13" s="11"/>
+      <c r="N13" s="12">
         <v>21227</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s" s="26">
         <v>26</v>
       </c>
-      <c r="B13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.12.1977</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="B14" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F14" s="34">
         <v>874737</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G14" t="s" s="37">
         <v>0</v>
       </c>
-      <c r="N13" s="1">
+      <c r="H14" s="11"/>
+      <c r="N14" s="12">
         <v>28474</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s" s="26">
         <v>26</v>
       </c>
-      <c r="B14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.12.1977</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="B15" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F15" s="34">
         <v>874735</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G15" t="s" s="37">
         <v>75</v>
       </c>
-      <c r="N14" s="1">
+      <c r="H15" s="11"/>
+      <c r="N15" s="12">
         <v>28474</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:30" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s" s="26">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15.12.1977</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="B16" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F16" s="34">
         <v>874733</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G16" t="s" s="37">
         <v>74</v>
       </c>
-      <c r="N15" s="1">
+      <c r="H16" s="11"/>
+      <c r="N16" s="12">
         <v>28474</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s" s="26">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>17.08.1988</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="B17" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" t="s" s="33">
         <v>73</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F17" s="34">
         <v>874737</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G17" t="s" s="37">
         <v>0</v>
       </c>
-      <c r="N16" s="1">
+      <c r="H17" s="11"/>
+      <c r="N17" s="12">
         <v>32372</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s" s="26">
         <v>28</v>
       </c>
-      <c r="B17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>17.08.1988</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="B18" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" t="s" s="33">
         <v>73</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="34">
         <v>874735</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G18" t="s" s="37">
         <v>75</v>
       </c>
-      <c r="N17" s="1">
+      <c r="H18" s="11"/>
+      <c r="N18" s="12">
         <v>32372</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s" s="26">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>17.08.1988</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="B19" s="10">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" t="s" s="33">
         <v>73</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F19" s="34">
         <v>874733</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G19" t="s" s="37">
         <v>74</v>
       </c>
-      <c r="N18" s="1">
+      <c r="H19" s="11"/>
+      <c r="N19" s="12">
         <v>32372</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DB53C3-3DE8-452D-A061-B42C08640916}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027DBE9-90F8-4510-9A2A-0DC7F76ECC31}">
+  <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B1:B10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="19.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="str">
-        <f>[1]Лист2!G1</f>
-        <v>Каргина Елена Геннадьевна</v>
+    <row r="1" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="2">
+        <v>17</v>
       </c>
       <c r="B1" s="6">
-        <f>[1]Лист2!H1</f>
-        <v>26862</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>66</v>
+        <f t="shared" ref="B1:B18" si="0">TEXT(N1, "ДД.ММ.ГГГГ")</f>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>69</v>
       </c>
       <c r="F1" s="8">
         <v>874737</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" t="s" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
+      <c r="N1" s="1">
+        <v>19647</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="2">
+        <v>17</v>
       </c>
       <c r="B2" s="6">
-        <v>26862</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>66</v>
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D2" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s" s="1">
+        <v>69</v>
       </c>
       <c r="F2" s="8">
         <v>874735</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
+      <c r="G2" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="N2" s="1">
+        <v>19647</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="2">
+        <v>17</v>
       </c>
       <c r="B3" s="6">
-        <v>26862</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>66</v>
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D3" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s" s="1">
+        <v>69</v>
       </c>
       <c r="F3" s="8">
         <v>874733</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="str">
-        <f>[1]Лист2!G4</f>
-        <v>Докучаев Сергей Александрович</v>
+      <c r="G3" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="N3" s="1">
+        <v>19647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="2">
+        <v>20</v>
       </c>
       <c r="B4" s="6">
-        <f>[1]Лист2!H4</f>
-        <v>22136</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D4" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="F4" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G4" t="s" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>21078</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D5" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="F5" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G5" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="N5" s="1">
+        <v>21078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D6" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="F6" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G6" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="N6" s="1">
+        <v>21078</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D7" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="F7" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>17351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D8" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="F8" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G8" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="N8" s="1">
+        <v>17351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D9" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="F9" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G9" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="N9" s="1">
+        <v>17351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D10" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="F10" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G10" t="s" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>21227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D11" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="F11" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G11" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="N11" s="1">
+        <v>21227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D12" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="F12" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G12" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="N12" s="1">
+        <v>21227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D13" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G13" t="s" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>28474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D14" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="F14" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G14" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="N14" s="1">
+        <v>28474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D15" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="F15" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G15" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="N15" s="1">
+        <v>28474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D16" t="s" s="1">
         <v>63</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="str">
-        <f>[1]Лист2!G5</f>
-        <v>Никитина Валентина Петровна</v>
-      </c>
-      <c r="B5" s="6">
-        <f>[1]Лист2!H5</f>
-        <v>19647</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="str">
-        <f>[1]Лист2!G6</f>
-        <v>Челищева Наталья Владимировна</v>
-      </c>
-      <c r="B6" s="6">
-        <f>[1]Лист2!H6</f>
-        <v>21078</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="str">
-        <f>[1]Лист2!G7</f>
-        <v>Закомлистова Раиса Федоровна</v>
-      </c>
-      <c r="B7" s="6">
-        <f>[1]Лист2!H7</f>
-        <v>17351</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="str">
-        <f>[1]Лист2!G8</f>
-        <v>Земерев Виктор Васильевич</v>
-      </c>
-      <c r="B8" s="6">
-        <f>[1]Лист2!H8</f>
-        <v>21227</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="str">
-        <f>[1]Лист2!G9</f>
-        <v>Аралкина Оксана Анатольевна</v>
-      </c>
-      <c r="B9" s="6">
-        <f>[1]Лист2!H9</f>
-        <v>28474</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="str">
-        <f>[1]Лист2!G10</f>
-        <v>Гайфуллина Лиана Римовна</v>
-      </c>
-      <c r="B10" s="6">
-        <f>[1]Лист2!H10</f>
+      <c r="E16" t="s" s="1">
+        <v>73</v>
+      </c>
+      <c r="F16" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G16" t="s" s="8">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
         <v>32372</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
+    </row>
+    <row r="17" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D17" t="s" s="1">
         <v>63</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E17" t="s" s="1">
         <v>73</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F17" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G17" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="N17" s="1">
+        <v>32372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="D18" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s" s="1">
+        <v>73</v>
+      </c>
+      <c r="F18" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G18" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="N18" s="1">
+        <v>32372</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1449,22 +1953,229 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DB53C3-3DE8-452D-A061-B42C08640916}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B10" sqref="B1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5">
+        <f>[1]Лист2!G1</f>
+      </c>
+      <c r="B1" s="6">
+        <f>[1]Лист2!H1</f>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="F1" s="8">
+        <v>874737</v>
+      </c>
+      <c r="G1" t="s" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>26862</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="F2" s="8">
+        <v>874735</v>
+      </c>
+      <c r="G2" t="s" s="8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>26862</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="F3" s="8">
+        <v>874733</v>
+      </c>
+      <c r="G3" t="s" s="8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <f>[1]Лист2!G4</f>
+      </c>
+      <c r="B4" s="6">
+        <f>[1]Лист2!H4</f>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <f>[1]Лист2!G5</f>
+      </c>
+      <c r="B5" s="6">
+        <f>[1]Лист2!H5</f>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <f>[1]Лист2!G6</f>
+      </c>
+      <c r="B6" s="6">
+        <f>[1]Лист2!H6</f>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <f>[1]Лист2!G7</f>
+      </c>
+      <c r="B7" s="6">
+        <f>[1]Лист2!H7</f>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <f>[1]Лист2!G8</f>
+      </c>
+      <c r="B8" s="6">
+        <f>[1]Лист2!H8</f>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <f>[1]Лист2!G9</f>
+      </c>
+      <c r="B9" s="6">
+        <f>[1]Лист2!H9</f>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <f>[1]Лист2!G10</f>
+      </c>
+      <c r="B10" s="6">
+        <f>[1]Лист2!H10</f>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE245E9-7BBB-4B60-A4DB-BD39DD0FE660}">
-  <dimension ref="A1:K24"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="36.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="11" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" customWidth="1"/>
+    <col min="10" max="10" width="60.6640625" customWidth="1"/>
+    <col min="11" max="11" width="34.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1499,7 +2210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +2221,7 @@
         <v>44067</v>
       </c>
       <c r="D2" s="4">
-        <v>0.44444444444444442</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E2">
         <v>1299807</v>
@@ -1534,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1569,7 +2280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1580,7 +2291,7 @@
         <v>44067</v>
       </c>
       <c r="D4" s="4">
-        <v>0.45833333333333331</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E4">
         <v>1299951</v>
@@ -1604,7 +2315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1639,7 +2350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1674,7 +2385,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1685,7 +2396,7 @@
         <v>44067</v>
       </c>
       <c r="D7" s="4">
-        <v>0.47916666666666669</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E7">
         <v>1299999</v>
@@ -1709,7 +2420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1744,7 +2455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1755,7 +2466,7 @@
         <v>44068</v>
       </c>
       <c r="D9" s="4">
-        <v>0.49305555555555558</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E9">
         <v>1300748</v>
@@ -1779,7 +2490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1814,7 +2525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1825,7 +2536,7 @@
         <v>44067</v>
       </c>
       <c r="D11" s="4">
-        <v>0.50694444444444442</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E11">
         <v>1300309</v>
@@ -1849,7 +2560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1860,7 +2571,7 @@
         <v>44068</v>
       </c>
       <c r="D12" s="4">
-        <v>0.51388888888888895</v>
+        <v>0.513888888888889</v>
       </c>
       <c r="E12">
         <v>1301451</v>
@@ -1881,7 +2592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1892,7 +2603,7 @@
         <v>44068</v>
       </c>
       <c r="D13" s="4">
-        <v>0.52083333333333337</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E13">
         <v>1301537</v>
@@ -1916,7 +2627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1927,7 +2638,7 @@
         <v>44068</v>
       </c>
       <c r="D14" s="4">
-        <v>0.52777777777777779</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E14">
         <v>1301574</v>
@@ -1951,7 +2662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1962,7 +2673,7 @@
         <v>44068</v>
       </c>
       <c r="D15" s="4">
-        <v>0.53472222222222221</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E15">
         <v>1301580</v>
@@ -1983,7 +2694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1994,7 +2705,7 @@
         <v>44068</v>
       </c>
       <c r="D16" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E16">
         <v>1301601</v>
@@ -2018,7 +2729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2740,7 @@
         <v>44068</v>
       </c>
       <c r="D17" s="4">
-        <v>0.54861111111111105</v>
+        <v>0.548611111111111</v>
       </c>
       <c r="E17">
         <v>1301621</v>
@@ -2053,7 +2764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2064,7 +2775,7 @@
         <v>44068</v>
       </c>
       <c r="D18" s="4">
-        <v>0.55555555555555558</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E18">
         <v>1301652</v>
@@ -2088,7 +2799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2123,7 +2834,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +2845,7 @@
         <v>44070</v>
       </c>
       <c r="D20" s="4">
-        <v>0.56944444444444442</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E20">
         <v>1304596</v>
@@ -2158,7 +2869,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2169,7 +2880,7 @@
         <v>44070</v>
       </c>
       <c r="D21" s="4">
-        <v>0.57638888888888895</v>
+        <v>0.576388888888889</v>
       </c>
       <c r="E21">
         <v>1304620</v>
@@ -2193,7 +2904,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2228,7 +2939,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -2263,7 +2974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
added two new parameters
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Documents\GitHub\promed-clicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728777EC-1791-455C-82A3-D0D956820214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EC172B-2811-4335-BC9B-EDACF32C0885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{6CCF5E32-90BF-4976-8CE3-9868609CAAE5}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'My Sheet'!$A$1:$H$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'My Sheet'!$A$1:$J$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="95">
   <si>
     <t>A06.09.005</t>
   </si>
@@ -291,13 +291,46 @@
   </si>
   <si>
     <t>РЕЗУЛЬТАТ</t>
+  </si>
+  <si>
+    <t>БАДАМШИН САЛАВАТ ЯНГАЛИЕВИЧ</t>
+  </si>
+  <si>
+    <t>D14.1</t>
+  </si>
+  <si>
+    <t>А06.09.005</t>
+  </si>
+  <si>
+    <t>А06.03.058</t>
+  </si>
+  <si>
+    <t>Домрачев Николай Никитич</t>
+  </si>
+  <si>
+    <t>C83.0</t>
+  </si>
+  <si>
+    <t>Федотова Людмила Ивановна</t>
+  </si>
+  <si>
+    <t>N85.0</t>
+  </si>
+  <si>
+    <t>ВРАЧ-ДИАГНОСТ</t>
+  </si>
+  <si>
+    <t>Ибрагимов Булат Айдарович</t>
+  </si>
+  <si>
+    <t>ДАТА</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +364,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="PT Sans Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="PT Sans Narrow"/>
       <family val="2"/>
@@ -497,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -606,10 +646,22 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -940,10 +992,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,13 +1007,15 @@
     <col min="5" max="5" width="10.7109375" style="10" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="10" customWidth="1"/>
-    <col min="9" max="13" width="8.85546875" style="10"/>
-    <col min="14" max="14" width="19.28515625" style="11" customWidth="1"/>
-    <col min="15" max="30" width="8.85546875" style="10"/>
+    <col min="8" max="8" width="40.7109375" style="10" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="10"/>
+    <col min="12" max="12" width="19.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="28" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="16" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="16" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>82</v>
       </c>
@@ -983,15 +1037,19 @@
       <c r="G1" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
       <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="L1" s="15"/>
       <c r="M1" s="14"/>
-      <c r="N1" s="15"/>
+      <c r="N1" s="14"/>
       <c r="O1" s="14"/>
       <c r="P1" s="14"/>
       <c r="Q1" s="14"/>
@@ -1006,444 +1064,442 @@
       <c r="Z1" s="14"/>
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-    </row>
-    <row r="2" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="38" t="str">
-        <f>TEXT(N2, "ДД.ММ.ГГГГ")</f>
-        <v>15.10.1953</v>
+        <v>84</v>
+      </c>
+      <c r="B2" s="39" t="str">
+        <f>TEXT(L2, "ДД.ММ.ГГГГ")</f>
+        <v>10.04.1958</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="26"/>
       <c r="E2" s="29" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="F2" s="30">
         <v>874737</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="N2" s="10">
-        <v>19647</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>17</v>
+        <v>86</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="43" t="str">
+        <f>TEXT(M2, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="L2" s="11">
+        <v>21285</v>
+      </c>
+      <c r="M2" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="B3" s="39" t="str">
-        <f t="shared" ref="B3:B19" si="0">TEXT(N3, "ДД.ММ.ГГГГ")</f>
-        <v>15.10.1953</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="31" t="s">
-        <v>69</v>
+        <f t="shared" ref="B3:B4" si="0">TEXT(L3, "ДД.ММ.ГГГГ")</f>
+        <v>10.04.1958</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="F3" s="32">
-        <v>874735</v>
+        <v>874739</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="N3" s="10">
-        <v>19647</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>17</v>
+        <v>87</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="43" t="str">
+        <f t="shared" ref="I3:I9" si="1">TEXT(M3, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="L3" s="11">
+        <v>21285</v>
+      </c>
+      <c r="M3" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="B4" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>15.10.1953</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="31" t="s">
-        <v>69</v>
+        <v>10.04.1958</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="F4" s="32">
-        <v>874733</v>
+        <v>874735</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="N4" s="10">
-        <v>19647</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="L4" s="11">
+        <v>21285</v>
+      </c>
+      <c r="M4" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>15.09.1957</v>
+        <v>88</v>
+      </c>
+      <c r="B5" s="38" t="str">
+        <f>TEXT(L5, "ДД.ММ.ГГГГ")</f>
+        <v>31.03.1955</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="28"/>
       <c r="E5" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="32">
+        <v>89</v>
+      </c>
+      <c r="F5" s="30">
         <v>874737</v>
       </c>
-      <c r="G5" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="N5" s="10">
-        <v>21078</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="L5" s="10">
+        <v>20179</v>
+      </c>
+      <c r="M5" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>15.09.1957</v>
+        <v>88</v>
+      </c>
+      <c r="B6" s="38" t="str">
+        <f>TEXT(L6, "ДД.ММ.ГГГГ")</f>
+        <v>31.03.1955</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
       <c r="E6" s="31" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="F6" s="32">
-        <v>874735</v>
+        <v>874739</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="N6" s="10">
-        <v>21078</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="L6" s="10">
+        <v>20179</v>
+      </c>
+      <c r="M6" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>15.09.1957</v>
+        <v>88</v>
+      </c>
+      <c r="B7" s="38" t="str">
+        <f>TEXT(L7, "ДД.ММ.ГГГГ")</f>
+        <v>31.03.1955</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28"/>
       <c r="E7" s="31" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="F7" s="32">
-        <v>874733</v>
+        <v>874735</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="N7" s="10">
-        <v>21078</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="L7" s="10">
+        <v>20179</v>
+      </c>
+      <c r="M7" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>03.07.1947</v>
+        <v>90</v>
+      </c>
+      <c r="B8" s="38" t="str">
+        <f>TEXT(L8, "ДД.ММ.ГГГГ")</f>
+        <v>29.09.1960</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
       <c r="E8" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="32">
+        <v>91</v>
+      </c>
+      <c r="F8" s="30">
         <v>874737</v>
       </c>
-      <c r="G8" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="N8" s="10">
-        <v>17351</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="L8" s="40">
+        <v>22188</v>
+      </c>
+      <c r="M8" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>03.07.1947</v>
+        <v>90</v>
+      </c>
+      <c r="B9" s="38" t="str">
+        <f>TEXT(L9, "ДД.ММ.ГГГГ")</f>
+        <v>29.09.1960</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="28"/>
       <c r="E9" s="31" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="F9" s="32">
-        <v>874735</v>
+        <v>874739</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="N9" s="10">
-        <v>17351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>03.07.1947</v>
+        <v>87</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>31.08.2020</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="L9" s="40">
+        <v>22188</v>
+      </c>
+      <c r="M9" s="43">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="38" t="str">
+        <f>TEXT(L10, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="28"/>
-      <c r="E10" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="32">
-        <v>874733</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="N10" s="10">
-        <v>17351</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>11.02.1958</v>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="9"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="38" t="str">
+        <f>TEXT(L11, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="28"/>
-      <c r="E11" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="32">
-        <v>874737</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="N11" s="10">
-        <v>21227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>11.02.1958</v>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="9"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="38" t="str">
+        <f>TEXT(L12, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="28"/>
-      <c r="E12" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="32">
-        <v>874735</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="N12" s="10">
-        <v>21227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>11.02.1958</v>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="9"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="38" t="str">
+        <f>TEXT(L13, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="28"/>
-      <c r="E13" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="32">
-        <v>874733</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="N13" s="10">
-        <v>21227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>15.12.1977</v>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="9"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="38" t="str">
+        <f>TEXT(L14, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="28"/>
-      <c r="E14" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="32">
-        <v>874737</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="N14" s="10">
-        <v>28474</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>15.12.1977</v>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="9"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="38" t="str">
+        <f>TEXT(L15, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="32">
-        <v>874735</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="N15" s="10">
-        <v>28474</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>15.12.1977</v>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="9"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="38" t="str">
+        <f>TEXT(L16, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
-      <c r="E16" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="32">
-        <v>874733</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="N16" s="10">
-        <v>28474</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>17.08.1988</v>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="9"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="38" t="str">
+        <f>TEXT(L17, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="28"/>
-      <c r="E17" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="32">
-        <v>874737</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="N17" s="10">
-        <v>32372</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>17.08.1988</v>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="9"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="38" t="str">
+        <f>TEXT(L18, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="32">
-        <v>874735</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="N18" s="10">
-        <v>32372</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>17.08.1988</v>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="9"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="38" t="str">
+        <f>TEXT(L19, "ДД.ММ.ГГГГ")</f>
+        <v>00.01.1900</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
-      <c r="E19" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="32">
-        <v>874733</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="N19" s="10">
-        <v>32372</v>
-      </c>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="9"/>
+      <c r="L19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
some govnokod due testing
running the script according to the codes in one xlsx line
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Documents\GitHub\promed-clicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA06F8-A90E-4199-9D1C-BD1549BCABD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2578FD9-267E-4610-B0FF-154758E3C3E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{6CCF5E32-90BF-4976-8CE3-9868609CAAE5}"/>
   </bookViews>
   <sheets>
-    <sheet name="My Sheet" sheetId="4" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
-    <sheet name="Лист1 (2)" sheetId="3" r:id="rId3"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId4"/>
+    <sheet name="My Sheet (2)" sheetId="5" r:id="rId1"/>
+    <sheet name="My Sheet" sheetId="4" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId3"/>
+    <sheet name="Лист1 (2)" sheetId="3" r:id="rId4"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'My Sheet'!$A$1:$J$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'My Sheet'!$A$1:$J$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'My Sheet (2)'!$A$1:$M$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="167">
   <si>
     <t>A06.09.005</t>
   </si>
@@ -293,9 +295,6 @@
     <t>РЕЗУЛЬТАТ</t>
   </si>
   <si>
-    <t>БАДАМШИН САЛАВАТ ЯНГАЛИЕВИЧ</t>
-  </si>
-  <si>
     <t>D14.1</t>
   </si>
   <si>
@@ -305,15 +304,9 @@
     <t>А06.03.058</t>
   </si>
   <si>
-    <t>Домрачев Николай Никитич</t>
-  </si>
-  <si>
     <t>C83.0</t>
   </si>
   <si>
-    <t>Федотова Людмила Ивановна</t>
-  </si>
-  <si>
     <t>N85.0</t>
   </si>
   <si>
@@ -324,13 +317,238 @@
   </si>
   <si>
     <t>ДАТА</t>
+  </si>
+  <si>
+    <t>ет</t>
+  </si>
+  <si>
+    <t>Расулов Радик Шамсутдинович</t>
+  </si>
+  <si>
+    <t>9279278240 (БД)</t>
+  </si>
+  <si>
+    <t>Новиков Николай Владимирович</t>
+  </si>
+  <si>
+    <t>9174365453 (БД)</t>
+  </si>
+  <si>
+    <t>АХМЕРОВ ЮРИЙ НИКОЛАЕВИЧ</t>
+  </si>
+  <si>
+    <t>9270812255 (БД)</t>
+  </si>
+  <si>
+    <t>ДАВЛЕТЯРОВ ФАНУС ГАББАСОВИЧ</t>
+  </si>
+  <si>
+    <t>9613570108 (БД)</t>
+  </si>
+  <si>
+    <t>Габитова Умугульсум Салимьяновна</t>
+  </si>
+  <si>
+    <t>9613703460 (БД)</t>
+  </si>
+  <si>
+    <t>ДЮСМЕТОВА АЛИЯ ИЛЮСОВНА</t>
+  </si>
+  <si>
+    <t>9371629297 (БД)</t>
+  </si>
+  <si>
+    <t>Субботкина Александра Петровна</t>
+  </si>
+  <si>
+    <t>9053597578 (БД)</t>
+  </si>
+  <si>
+    <t>ГАУЗ РКОД МЗ РБ, ОНКО-УРОЛОГ</t>
+  </si>
+  <si>
+    <t>Коротков Владимир Александрович</t>
+  </si>
+  <si>
+    <t>9273298877 (БД)</t>
+  </si>
+  <si>
+    <t>Хазиев А Р</t>
+  </si>
+  <si>
+    <t>Костюкевич Елена Петровна</t>
+  </si>
+  <si>
+    <t>9871060727 (БД)</t>
+  </si>
+  <si>
+    <t>Шагимарданова Ольга Михайловна</t>
+  </si>
+  <si>
+    <t>9613581026 (БД)</t>
+  </si>
+  <si>
+    <t>ГАУЗ РКОД МЗ РБ, ОБЩИЙ ОНКОЛОГ (1 пол)</t>
+  </si>
+  <si>
+    <t>Коробкина Татьяна Валериановна</t>
+  </si>
+  <si>
+    <t>3475023116 (БД)</t>
+  </si>
+  <si>
+    <t>Фархутдинова Е Ф</t>
+  </si>
+  <si>
+    <t>Казаченко Виктор Лаврентьевич</t>
+  </si>
+  <si>
+    <t>0002442637 (БД)</t>
+  </si>
+  <si>
+    <t>Мухаметдинова Райса Юсуповна</t>
+  </si>
+  <si>
+    <t>3477028125 (БД)</t>
+  </si>
+  <si>
+    <t>Афзалетдинова Зиля Радиковна</t>
+  </si>
+  <si>
+    <t>9273012307 (БД)</t>
+  </si>
+  <si>
+    <t>Мухамедьянов Валерий Анатолеевич</t>
+  </si>
+  <si>
+    <t>9174150248 (БД)</t>
+  </si>
+  <si>
+    <t>Закиров Рашит Исмагилович</t>
+  </si>
+  <si>
+    <t>9174401679 (БД)</t>
+  </si>
+  <si>
+    <t>ГАУЗ РКОД МЗ РБ, 1.ПАЛЛИАТИВНАЯ ПОМОЩЬ</t>
+  </si>
+  <si>
+    <t>МИХАЙЛОВ СЕРГЕЙ ВЛАДИМИРОВИЧ</t>
+  </si>
+  <si>
+    <t>9174353729 (БД)</t>
+  </si>
+  <si>
+    <t>МЕЛЬНИЧУК А В</t>
+  </si>
+  <si>
+    <t>ЛЫСКОВА ГАЛИНА ВАСИЛЬЕВНА</t>
+  </si>
+  <si>
+    <t>9173642103 (БД)</t>
+  </si>
+  <si>
+    <t>Кудряшов А А</t>
+  </si>
+  <si>
+    <t>Акбатыров Миняй Иманбаевич</t>
+  </si>
+  <si>
+    <t>9273248153 (БД)</t>
+  </si>
+  <si>
+    <t>Нечитайло Нина Яновна</t>
+  </si>
+  <si>
+    <t>9174714456 (БД)</t>
+  </si>
+  <si>
+    <t>НУГУМАНОВА ДИНА ГАЙНУТДИНОВНА</t>
+  </si>
+  <si>
+    <t>+79174241257 (портал самозаписи); 9174241257 (БД)</t>
+  </si>
+  <si>
+    <t>Валиахметова Ч Х</t>
+  </si>
+  <si>
+    <t>Тугалуков Владимир Михайлович</t>
+  </si>
+  <si>
+    <t>9279679021 (БД)</t>
+  </si>
+  <si>
+    <t>Белихова Роза Абдурахмановна</t>
+  </si>
+  <si>
+    <t>9050043225 (БД)</t>
+  </si>
+  <si>
+    <t>C32.3</t>
+  </si>
+  <si>
+    <t>C32.9</t>
+  </si>
+  <si>
+    <t>D23.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D12.5 </t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>D06.7</t>
+  </si>
+  <si>
+    <t>N87.1</t>
+  </si>
+  <si>
+    <t>C61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D48.6 </t>
+  </si>
+  <si>
+    <t>D21.3</t>
+  </si>
+  <si>
+    <t>C67.9</t>
+  </si>
+  <si>
+    <t>C50.4</t>
+  </si>
+  <si>
+    <t>D12.8</t>
+  </si>
+  <si>
+    <t>C34.8</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>D40.9</t>
+  </si>
+  <si>
+    <t>C54.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20 </t>
+  </si>
+  <si>
+    <t>C50.2</t>
+  </si>
+  <si>
+    <t>А06.30.005.001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +591,27 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="PT Sans Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -537,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,6 +907,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -994,14 +1269,753 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5082DBDE-3286-4633-AF7C-B43FDC366AA9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AI25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="37" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="10" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="10" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="10"/>
+    <col min="15" max="15" width="19.28515625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="23" width="8.85546875" style="10"/>
+    <col min="24" max="24" width="30.42578125" style="10" customWidth="1"/>
+    <col min="25" max="29" width="8.85546875" style="10"/>
+    <col min="30" max="30" width="20.7109375" style="10" customWidth="1"/>
+    <col min="31" max="31" width="31.5703125" style="10" customWidth="1"/>
+    <col min="32" max="32" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="16" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+    </row>
+    <row r="2" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="55" t="str">
+        <f>TEXT(O2, "ДД.ММ.ГГГГ")</f>
+        <v>04.12.1954</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="55" t="str">
+        <f>TEXT(P2, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="59">
+        <v>874737</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="59">
+        <v>874735</v>
+      </c>
+      <c r="K2" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="59">
+        <v>874733</v>
+      </c>
+      <c r="M2" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="11">
+        <v>20062</v>
+      </c>
+      <c r="P2" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T2" s="11"/>
+      <c r="U2" s="46"/>
+      <c r="Y2" s="11"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
+    </row>
+    <row r="3" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="55" t="str">
+        <f t="shared" ref="B3:B19" si="0">TEXT(O3, "ДД.ММ.ГГГГ")</f>
+        <v>10.04.1958</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="55" t="str">
+        <f>TEXT(P3, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="O3" s="11">
+        <v>21285</v>
+      </c>
+      <c r="P3" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T3" s="11"/>
+      <c r="U3" s="46"/>
+      <c r="Y3" s="11"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+    </row>
+    <row r="4" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>10.04.1958</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="55" t="str">
+        <f>TEXT(P4, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G4" s="58"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="O4" s="11">
+        <v>21285</v>
+      </c>
+      <c r="P4" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T4" s="11"/>
+      <c r="U4" s="46"/>
+      <c r="Y4" s="11"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="47"/>
+    </row>
+    <row r="5" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>31.03.1955</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="55" t="str">
+        <f>TEXT(P5, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="O5" s="10">
+        <v>20179</v>
+      </c>
+      <c r="P5" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T5" s="11"/>
+      <c r="U5" s="46"/>
+      <c r="Y5" s="11"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+    </row>
+    <row r="6" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>31.03.1955</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="55" t="str">
+        <f>TEXT(P6, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="O6" s="10">
+        <v>20179</v>
+      </c>
+      <c r="P6" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T6" s="11"/>
+      <c r="U6" s="46"/>
+      <c r="Y6" s="11"/>
+      <c r="AD6" s="47"/>
+      <c r="AE6" s="47"/>
+      <c r="AF6" s="47"/>
+      <c r="AG6" s="47"/>
+      <c r="AH6" s="47"/>
+      <c r="AI6" s="47"/>
+    </row>
+    <row r="7" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>31.03.1955</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="55" t="str">
+        <f>TEXT(P7, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G7" s="58"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="O7" s="10">
+        <v>20179</v>
+      </c>
+      <c r="P7" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T7" s="11"/>
+      <c r="U7" s="46"/>
+      <c r="Y7" s="11"/>
+      <c r="AD7" s="47"/>
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="47"/>
+      <c r="AI7" s="47"/>
+    </row>
+    <row r="8" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>29.09.1960</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="55" t="str">
+        <f>TEXT(P8, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="O8" s="39">
+        <v>22188</v>
+      </c>
+      <c r="P8" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T8" s="11"/>
+      <c r="U8" s="46"/>
+      <c r="Y8" s="11"/>
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="47"/>
+    </row>
+    <row r="9" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="54"/>
+      <c r="B9" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>29.09.1960</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="55" t="str">
+        <f>TEXT(P9, "ДД.ММ.ГГГГ")</f>
+        <v>31.08.2020</v>
+      </c>
+      <c r="G9" s="58"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="O9" s="39">
+        <v>22188</v>
+      </c>
+      <c r="P9" s="41">
+        <v>44074</v>
+      </c>
+      <c r="T9" s="11"/>
+      <c r="U9" s="46"/>
+      <c r="Y9" s="11"/>
+      <c r="AD9" s="47"/>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="47"/>
+      <c r="AG9" s="47"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+    </row>
+    <row r="10" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="54"/>
+      <c r="B10" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="O10" s="10"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="46"/>
+      <c r="Y10" s="11"/>
+      <c r="AD10" s="47"/>
+      <c r="AE10" s="47"/>
+      <c r="AF10" s="47"/>
+      <c r="AG10" s="47"/>
+      <c r="AH10" s="47"/>
+      <c r="AI10" s="47"/>
+    </row>
+    <row r="11" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="O11" s="10"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="46"/>
+      <c r="Y11" s="11"/>
+      <c r="AD11" s="47"/>
+      <c r="AE11" s="47"/>
+      <c r="AF11" s="47"/>
+      <c r="AG11" s="47"/>
+      <c r="AH11" s="47"/>
+      <c r="AI11" s="47"/>
+    </row>
+    <row r="12" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C12" s="56"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="O12" s="10"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="46"/>
+      <c r="Y12" s="11"/>
+      <c r="AD12" s="47"/>
+      <c r="AE12" s="47"/>
+      <c r="AF12" s="47"/>
+      <c r="AG12" s="47"/>
+      <c r="AH12" s="47"/>
+      <c r="AI12" s="47"/>
+    </row>
+    <row r="13" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="O13" s="10"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="46"/>
+      <c r="Y13" s="11"/>
+      <c r="AD13" s="47"/>
+      <c r="AE13" s="47"/>
+      <c r="AF13" s="47"/>
+      <c r="AG13" s="47"/>
+      <c r="AH13" s="47"/>
+      <c r="AI13" s="47"/>
+    </row>
+    <row r="14" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+      <c r="B14" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="O14" s="10"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="46"/>
+      <c r="Y14" s="11"/>
+      <c r="AD14" s="47"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
+      <c r="AG14" s="47"/>
+      <c r="AH14" s="47"/>
+      <c r="AI14" s="47"/>
+    </row>
+    <row r="15" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C15" s="56"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="O15" s="10"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="46"/>
+      <c r="Y15" s="11"/>
+      <c r="AD15" s="47"/>
+      <c r="AE15" s="47"/>
+      <c r="AF15" s="47"/>
+      <c r="AG15" s="47"/>
+      <c r="AH15" s="47"/>
+      <c r="AI15" s="47"/>
+    </row>
+    <row r="16" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C16" s="56"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="O16" s="10"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="46"/>
+      <c r="Y16" s="11"/>
+      <c r="AD16" s="47"/>
+      <c r="AE16" s="47"/>
+      <c r="AF16" s="47"/>
+      <c r="AG16" s="47"/>
+      <c r="AH16" s="47"/>
+      <c r="AI16" s="47"/>
+    </row>
+    <row r="17" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="O17" s="10"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="46"/>
+      <c r="Y17" s="11"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="47"/>
+      <c r="AH17" s="47"/>
+      <c r="AI17" s="47"/>
+    </row>
+    <row r="18" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="O18" s="10"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="46"/>
+      <c r="Y18" s="11"/>
+      <c r="AD18" s="47"/>
+      <c r="AE18" s="47"/>
+      <c r="AF18" s="47"/>
+      <c r="AG18" s="47"/>
+      <c r="AH18" s="47"/>
+      <c r="AI18" s="47"/>
+    </row>
+    <row r="19" spans="1:35" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+      <c r="B19" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>00.01.1900</v>
+      </c>
+      <c r="C19" s="56"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="O19" s="10"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="46"/>
+      <c r="Y19" s="11"/>
+      <c r="AD19" s="47"/>
+      <c r="AE19" s="47"/>
+      <c r="AF19" s="48"/>
+      <c r="AG19" s="48"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="T20" s="11"/>
+      <c r="U20" s="46"/>
+      <c r="Y20" s="11"/>
+      <c r="AD20" s="47"/>
+      <c r="AE20" s="47"/>
+      <c r="AF20" s="47"/>
+      <c r="AG20" s="47"/>
+      <c r="AH20" s="47"/>
+      <c r="AI20" s="47"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="T21" s="11"/>
+      <c r="U21" s="46"/>
+      <c r="Y21" s="11"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="T22" s="11"/>
+      <c r="U22" s="46"/>
+      <c r="Y22" s="11"/>
+      <c r="AD22" s="47"/>
+      <c r="AE22" s="47"/>
+      <c r="AF22" s="49"/>
+      <c r="AG22" s="47"/>
+      <c r="AH22" s="47"/>
+      <c r="AI22" s="47"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="T23" s="11"/>
+      <c r="U23" s="46"/>
+      <c r="Y23" s="11"/>
+      <c r="AD23" s="47"/>
+      <c r="AE23" s="47"/>
+      <c r="AF23" s="47"/>
+      <c r="AG23" s="47"/>
+      <c r="AH23" s="47"/>
+      <c r="AI23" s="47"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="T24" s="11"/>
+      <c r="U24" s="46"/>
+      <c r="Y24" s="11"/>
+      <c r="AD24" s="47"/>
+      <c r="AE24" s="47"/>
+      <c r="AF24" s="47"/>
+      <c r="AG24" s="47"/>
+      <c r="AH24" s="47"/>
+      <c r="AI24" s="47"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AF25" s="47"/>
+      <c r="AG25" s="48"/>
+      <c r="AH25" s="47"/>
+      <c r="AI25" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="31" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C91358-37E6-4149-BBCE-8F9D3F17590A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,10 +2032,15 @@
     <col min="11" max="11" width="8.85546875" style="10"/>
     <col min="12" max="12" width="19.28515625" style="11" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="28" width="8.85546875" style="10"/>
+    <col min="14" max="20" width="8.85546875" style="10"/>
+    <col min="21" max="21" width="30.42578125" style="10" customWidth="1"/>
+    <col min="22" max="26" width="8.85546875" style="10"/>
+    <col min="27" max="27" width="20.7109375" style="10" customWidth="1"/>
+    <col min="28" max="28" width="31.5703125" style="10" customWidth="1"/>
+    <col min="29" max="29" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="16" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="16" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>82</v>
       </c>
@@ -1044,10 +2063,10 @@
         <v>80</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>83</v>
@@ -1071,10 +2090,8 @@
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
     </row>
-    <row r="2" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>84</v>
-      </c>
+    <row r="2" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
       <c r="B2" s="43" t="str">
         <f>TEXT(L2, "ДД.ММ.ГГГГ")</f>
         <v>10.04.1958</v>
@@ -1082,16 +2099,16 @@
       <c r="C2" s="25"/>
       <c r="D2" s="26"/>
       <c r="E2" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="30">
         <v>874737</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I2" s="42" t="str">
         <f t="shared" ref="I2:I9" si="0">TEXT(M2, "ДД.ММ.ГГГГ")</f>
@@ -1104,11 +2121,51 @@
       <c r="M2" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>84</v>
-      </c>
+      <c r="O2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>44069</v>
+      </c>
+      <c r="R2" s="46">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="S2" s="10">
+        <v>1303219</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="V2" s="11">
+        <v>20062</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA2" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB2" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
       <c r="B3" s="43" t="str">
         <f t="shared" ref="B3:B4" si="1">TEXT(L3, "ДД.ММ.ГГГГ")</f>
         <v>10.04.1958</v>
@@ -1116,16 +2173,16 @@
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="E3" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="32">
         <v>874739</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I3" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1138,11 +2195,51 @@
       <c r="M3" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>84</v>
-      </c>
+      <c r="O3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>44076</v>
+      </c>
+      <c r="R3" s="46">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="S3" s="10">
+        <v>1311731</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="V3" s="11">
+        <v>28778</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA3" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB3" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
       <c r="B4" s="43" t="str">
         <f t="shared" si="1"/>
         <v>10.04.1958</v>
@@ -1150,7 +2247,7 @@
       <c r="C4" s="25"/>
       <c r="D4" s="26"/>
       <c r="E4" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="32">
         <v>874735</v>
@@ -1159,7 +2256,7 @@
         <v>67</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I4" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1172,11 +2269,63 @@
       <c r="M4" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>88</v>
-      </c>
+      <c r="O4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>44071</v>
+      </c>
+      <c r="R4" s="46">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="S4" s="10">
+        <v>1306221</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="V4" s="11">
+        <v>20845</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA4" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB4" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC4" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD4" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE4" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF4" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
       <c r="B5" s="38" t="str">
         <f t="shared" ref="B5:B19" si="2">TEXT(L5, "ДД.ММ.ГГГГ")</f>
         <v>31.03.1955</v>
@@ -1184,16 +2333,16 @@
       <c r="C5" s="27"/>
       <c r="D5" s="28"/>
       <c r="E5" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F5" s="30">
         <v>874737</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I5" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1206,11 +2355,63 @@
       <c r="M5" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>88</v>
-      </c>
+      <c r="O5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>44071</v>
+      </c>
+      <c r="R5" s="46">
+        <v>0.4375</v>
+      </c>
+      <c r="S5" s="10">
+        <v>1306373</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="V5" s="11">
+        <v>17715</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA5" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB5" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC5" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD5" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE5" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF5" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
       <c r="B6" s="38" t="str">
         <f t="shared" si="2"/>
         <v>31.03.1955</v>
@@ -1218,16 +2419,16 @@
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
       <c r="E6" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F6" s="32">
         <v>874739</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I6" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1240,11 +2441,63 @@
       <c r="M6" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>88</v>
-      </c>
+      <c r="O6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>44072</v>
+      </c>
+      <c r="R6" s="46">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="S6" s="10">
+        <v>1306616</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="V6" s="11">
+        <v>15436</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA6" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB6" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC6" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD6" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE6" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF6" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
       <c r="B7" s="38" t="str">
         <f t="shared" si="2"/>
         <v>31.03.1955</v>
@@ -1252,7 +2505,7 @@
       <c r="C7" s="27"/>
       <c r="D7" s="28"/>
       <c r="E7" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" s="32">
         <v>874735</v>
@@ -1261,7 +2514,7 @@
         <v>67</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I7" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1274,11 +2527,63 @@
       <c r="M7" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>90</v>
-      </c>
+      <c r="O7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>44074</v>
+      </c>
+      <c r="R7" s="46">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="S7" s="10">
+        <v>1308175</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="V7" s="11">
+        <v>32745</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA7" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB7" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC7" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD7" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE7" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF7" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
       <c r="B8" s="38" t="str">
         <f t="shared" si="2"/>
         <v>29.09.1960</v>
@@ -1286,16 +2591,16 @@
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
       <c r="E8" s="31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F8" s="30">
         <v>874737</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I8" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1308,11 +2613,63 @@
       <c r="M8" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>90</v>
-      </c>
+      <c r="O8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R8" s="46">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="S8" s="10">
+        <v>1312753</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="V8" s="11">
+        <v>17069</v>
+      </c>
+      <c r="W8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="X8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z8" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA8" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB8" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC8" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD8" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE8" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF8" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
       <c r="B9" s="38" t="str">
         <f t="shared" si="2"/>
         <v>29.09.1960</v>
@@ -1320,16 +2677,16 @@
       <c r="C9" s="27"/>
       <c r="D9" s="28"/>
       <c r="E9" s="31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F9" s="32">
         <v>874739</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I9" s="42" t="str">
         <f t="shared" si="0"/>
@@ -1342,8 +2699,62 @@
       <c r="M9" s="41">
         <v>44074</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>44075</v>
+      </c>
+      <c r="R9" s="46">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="S9" s="10">
+        <v>1309022</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="V9" s="11">
+        <v>19063</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA9" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB9" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC9" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD9" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE9" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF9" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1358,8 +2769,62 @@
       <c r="I10" s="40"/>
       <c r="J10" s="9"/>
       <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>44075</v>
+      </c>
+      <c r="R10" s="46">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="S10" s="10">
+        <v>1309440</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="V10" s="11">
+        <v>30913</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="X10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z10" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA10" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB10" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC10" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD10" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE10" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF10" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1374,8 +2839,62 @@
       <c r="I11" s="40"/>
       <c r="J11" s="9"/>
       <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>44075</v>
+      </c>
+      <c r="R11" s="46">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="S11" s="10">
+        <v>1309877</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="V11" s="11">
+        <v>29448</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="X11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA11" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB11" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC11" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD11" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE11" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF11" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1390,8 +2909,62 @@
       <c r="I12" s="40"/>
       <c r="J12" s="9"/>
       <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>44076</v>
+      </c>
+      <c r="R12" s="46">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="S12" s="10">
+        <v>1311019</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="V12" s="11">
+        <v>30134</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="X12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA12" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB12" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC12" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD12" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE12" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF12" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1406,8 +2979,62 @@
       <c r="I13" s="40"/>
       <c r="J13" s="9"/>
       <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>44076</v>
+      </c>
+      <c r="R13" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="S13" s="10">
+        <v>1311144</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="V13" s="11">
+        <v>20058</v>
+      </c>
+      <c r="W13" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="X13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z13" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA13" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB13" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC13" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD13" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE13" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF13" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1422,8 +3049,62 @@
       <c r="I14" s="40"/>
       <c r="J14" s="9"/>
       <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>44076</v>
+      </c>
+      <c r="R14" s="46">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="S14" s="10">
+        <v>1311678</v>
+      </c>
+      <c r="T14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="V14" s="11">
+        <v>19392</v>
+      </c>
+      <c r="W14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="X14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z14" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA14" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB14" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC14" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD14" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE14" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF14" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1438,8 +3119,62 @@
       <c r="I15" s="40"/>
       <c r="J15" s="9"/>
       <c r="L15" s="10"/>
-    </row>
-    <row r="16" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>44076</v>
+      </c>
+      <c r="R15" s="46">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="S15" s="10">
+        <v>1311688</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="V15" s="11">
+        <v>22246</v>
+      </c>
+      <c r="W15" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="X15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA15" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB15" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC15" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD15" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE15" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF15" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1454,8 +3189,62 @@
       <c r="I16" s="40"/>
       <c r="J16" s="9"/>
       <c r="L16" s="10"/>
-    </row>
-    <row r="17" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>44076</v>
+      </c>
+      <c r="R16" s="46">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="S16" s="10">
+        <v>1312029</v>
+      </c>
+      <c r="T16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="V16" s="11">
+        <v>21992</v>
+      </c>
+      <c r="W16" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="X16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA16" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB16" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC16" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD16" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE16" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF16" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1470,8 +3259,62 @@
       <c r="I17" s="40"/>
       <c r="J17" s="9"/>
       <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R17" s="46">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="S17" s="10">
+        <v>1312781</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="V17" s="11">
+        <v>20653</v>
+      </c>
+      <c r="W17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="X17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z17" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA17" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB17" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC17" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD17" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE17" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF17" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1486,8 +3329,62 @@
       <c r="I18" s="40"/>
       <c r="J18" s="9"/>
       <c r="L18" s="10"/>
-    </row>
-    <row r="19" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R18" s="46">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="S18" s="10">
+        <v>1312842</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="V18" s="11">
+        <v>18667</v>
+      </c>
+      <c r="W18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="X18" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y18" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z18" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA18" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB18" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC18" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD18" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE18" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF18" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="38" t="str">
         <f t="shared" si="2"/>
@@ -1502,6 +3399,348 @@
       <c r="I19" s="40"/>
       <c r="J19" s="9"/>
       <c r="L19" s="10"/>
+      <c r="O19" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R19" s="46">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="S19" s="10">
+        <v>1312866</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="V19" s="11">
+        <v>21792</v>
+      </c>
+      <c r="W19" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="X19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y19" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z19" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA19" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB19" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC19" s="48">
+        <v>874739</v>
+      </c>
+      <c r="AD19" s="48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O20" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R20" s="46">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="S20" s="10">
+        <v>1313147</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="V20" s="11">
+        <v>21116</v>
+      </c>
+      <c r="W20" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="X20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z20" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA20" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB20" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC20" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD20" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE20" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF20" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R21" s="46">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="S21" s="10">
+        <v>1313198</v>
+      </c>
+      <c r="T21" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="V21" s="11">
+        <v>18433</v>
+      </c>
+      <c r="W21" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="X21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA21" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB21" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC21" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD21" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE21" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF21" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R22" s="46">
+        <v>0.5625</v>
+      </c>
+      <c r="S22" s="10">
+        <v>1313247</v>
+      </c>
+      <c r="T22" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="U22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="V22" s="11">
+        <v>21396</v>
+      </c>
+      <c r="W22" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y22" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z22" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA22" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB22" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC22" s="49">
+        <v>874736</v>
+      </c>
+      <c r="AD22" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE22" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF22" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R23" s="46">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="S23" s="10">
+        <v>1313344</v>
+      </c>
+      <c r="T23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="V23" s="11">
+        <v>20786</v>
+      </c>
+      <c r="W23" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="X23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z23" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA23" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB23" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC23" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD23" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE23" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF23" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>44077</v>
+      </c>
+      <c r="R24" s="46">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="S24" s="10">
+        <v>1313462</v>
+      </c>
+      <c r="T24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U24" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="V24" s="11">
+        <v>22272</v>
+      </c>
+      <c r="W24" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="X24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z24" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA24" s="47">
+        <v>874737</v>
+      </c>
+      <c r="AB24" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC24" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AD24" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE24" s="47">
+        <v>874733</v>
+      </c>
+      <c r="AF24" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AC25" s="47">
+        <v>874739</v>
+      </c>
+      <c r="AD25" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE25" s="47">
+        <v>874735</v>
+      </c>
+      <c r="AF25" s="47" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1509,7 +3748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027DBE9-90F8-4510-9A2A-0DC7F76ECC31}">
   <dimension ref="A1:N18"/>
   <sheetViews>
@@ -1968,7 +4207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DB53C3-3DE8-452D-A061-B42C08640916}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -2175,7 +4414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE245E9-7BBB-4B60-A4DB-BD39DD0FE660}">
   <dimension ref="A1:K24"/>
   <sheetViews>

</xml_diff>